<commit_message>
is it fast enough?
</commit_message>
<xml_diff>
--- a/graphs/results.xlsx
+++ b/graphs/results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -737,6 +737,461 @@
       </c>
       <c r="K8" t="n">
         <v>2.266666666666667</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>10</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>90</v>
+      </c>
+      <c r="E9" t="n">
+        <v>820000</v>
+      </c>
+      <c r="F9" t="n">
+        <v>681972</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.08888888888888889</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.175</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>50</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2946</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2164</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.3875</v>
+      </c>
+      <c r="J10" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="K10" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>8</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>36</v>
+      </c>
+      <c r="E11" t="n">
+        <v>340</v>
+      </c>
+      <c r="F11" t="n">
+        <v>228</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.2777777777777778</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.4380952380952381</v>
+      </c>
+      <c r="J11" t="n">
+        <v>7.076923076923077</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2.769230769230769</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>14</v>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>70</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3923</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2814</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.3035714285714285</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2.428571428571428</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1.928571428571429</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>14</v>
+      </c>
+      <c r="B13" t="n">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>98</v>
+      </c>
+      <c r="E13" t="n">
+        <v>101131</v>
+      </c>
+      <c r="F13" t="n">
+        <v>78741</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.2103174603174603</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2.523809523809524</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1.619047619047619</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" t="n">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>56</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1538</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1085</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.4047619047619048</v>
+      </c>
+      <c r="J14" t="n">
+        <v>4.857142857142857</v>
+      </c>
+      <c r="K14" t="n">
+        <v>2.095238095238095</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>8</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>126</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1597600</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1329226</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.1629464285714286</v>
+      </c>
+      <c r="J15" t="n">
+        <v>2.607142857142857</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1.535714285714286</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>8</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>70</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3194</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2254</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.3214285714285715</v>
+      </c>
+      <c r="J16" t="n">
+        <v>5.142857142857143</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1.928571428571429</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>14</v>
+      </c>
+      <c r="B17" t="n">
+        <v>8</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" t="n">
+        <v>50</v>
+      </c>
+      <c r="E17" t="n">
+        <v>435</v>
+      </c>
+      <c r="F17" t="n">
+        <v>309</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.5257731958762887</v>
+      </c>
+      <c r="J17" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K17" t="n">
+        <v>2.555555555555555</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>14</v>
+      </c>
+      <c r="B18" t="n">
+        <v>10</v>
+      </c>
+      <c r="C18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" t="n">
+        <v>48</v>
+      </c>
+      <c r="E18" t="n">
+        <v>849</v>
+      </c>
+      <c r="F18" t="n">
+        <v>541</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.4693877551020408</v>
+      </c>
+      <c r="J18" t="n">
+        <v>9.470588235294118</v>
+      </c>
+      <c r="K18" t="n">
+        <v>2.823529411764706</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>80</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2224</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1718</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.296875</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2.375</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1.8125</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" t="n">
+        <v>6</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>112</v>
+      </c>
+      <c r="E20" t="n">
+        <v>139587</v>
+      </c>
+      <c r="F20" t="n">
+        <v>108916</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.2048611111111111</v>
+      </c>
+      <c r="J20" t="n">
+        <v>2.458333333333333</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1.583333333333333</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>16</v>
+      </c>
+      <c r="B21" t="n">
+        <v>6</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" t="n">
+        <v>64</v>
+      </c>
+      <c r="E21" t="n">
+        <v>809</v>
+      </c>
+      <c r="F21" t="n">
+        <v>606</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.3680555555555556</v>
+      </c>
+      <c r="J21" t="n">
+        <v>4.416666666666667</v>
+      </c>
+      <c r="K21" t="n">
+        <v>2.041666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -826,7 +1281,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1169,6 +1624,461 @@
       </c>
       <c r="K9" t="n">
         <v>1.65</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>50</v>
+      </c>
+      <c r="E10" t="n">
+        <v>9296</v>
+      </c>
+      <c r="F10" t="n">
+        <v>6497</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.3875</v>
+      </c>
+      <c r="J10" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="K10" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>8</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>36</v>
+      </c>
+      <c r="E11" t="n">
+        <v>146</v>
+      </c>
+      <c r="F11" t="n">
+        <v>108</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.4380952380952381</v>
+      </c>
+      <c r="J11" t="n">
+        <v>7.076923076923077</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2.769230769230769</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>14</v>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>70</v>
+      </c>
+      <c r="E12" t="n">
+        <v>815</v>
+      </c>
+      <c r="F12" t="n">
+        <v>629</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.3035714285714285</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2.428571428571428</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1.928571428571429</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>14</v>
+      </c>
+      <c r="B13" t="n">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>98</v>
+      </c>
+      <c r="E13" t="n">
+        <v>614</v>
+      </c>
+      <c r="F13" t="n">
+        <v>416</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.2103174603174603</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2.523809523809524</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1.619047619047619</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" t="n">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>56</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1160</v>
+      </c>
+      <c r="F14" t="n">
+        <v>758</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.03571428571428571</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.4047619047619048</v>
+      </c>
+      <c r="J14" t="n">
+        <v>4.857142857142857</v>
+      </c>
+      <c r="K14" t="n">
+        <v>2.095238095238095</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>8</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>126</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1597600</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1329475</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.01587301587301587</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.1629464285714286</v>
+      </c>
+      <c r="J15" t="n">
+        <v>2.607142857142857</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1.535714285714286</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>8</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>70</v>
+      </c>
+      <c r="E16" t="n">
+        <v>813</v>
+      </c>
+      <c r="F16" t="n">
+        <v>566</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.3214285714285715</v>
+      </c>
+      <c r="J16" t="n">
+        <v>5.142857142857143</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1.928571428571429</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>14</v>
+      </c>
+      <c r="B17" t="n">
+        <v>8</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" t="n">
+        <v>50</v>
+      </c>
+      <c r="E17" t="n">
+        <v>435</v>
+      </c>
+      <c r="F17" t="n">
+        <v>286</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.5257731958762887</v>
+      </c>
+      <c r="J17" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K17" t="n">
+        <v>2.555555555555555</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>14</v>
+      </c>
+      <c r="B18" t="n">
+        <v>10</v>
+      </c>
+      <c r="C18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" t="n">
+        <v>48</v>
+      </c>
+      <c r="E18" t="n">
+        <v>317</v>
+      </c>
+      <c r="F18" t="n">
+        <v>255</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.04166666666666666</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.4693877551020408</v>
+      </c>
+      <c r="J18" t="n">
+        <v>9.470588235294118</v>
+      </c>
+      <c r="K18" t="n">
+        <v>2.823529411764706</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>80</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1169</v>
+      </c>
+      <c r="F19" t="n">
+        <v>862</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.296875</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2.375</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1.8125</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" t="n">
+        <v>6</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>112</v>
+      </c>
+      <c r="E20" t="n">
+        <v>129252</v>
+      </c>
+      <c r="F20" t="n">
+        <v>100688</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.2048611111111111</v>
+      </c>
+      <c r="J20" t="n">
+        <v>2.458333333333333</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1.583333333333333</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>16</v>
+      </c>
+      <c r="B21" t="n">
+        <v>6</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" t="n">
+        <v>64</v>
+      </c>
+      <c r="E21" t="n">
+        <v>564</v>
+      </c>
+      <c r="F21" t="n">
+        <v>392</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.3680555555555556</v>
+      </c>
+      <c r="J21" t="n">
+        <v>4.416666666666667</v>
+      </c>
+      <c r="K21" t="n">
+        <v>2.041666666666667</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>16</v>
+      </c>
+      <c r="B22" t="n">
+        <v>8</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>144</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1220</v>
+      </c>
+      <c r="F22" t="n">
+        <v>914</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.16015625</v>
+      </c>
+      <c r="J22" t="n">
+        <v>2.5625</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>
@@ -1182,7 +2092,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1525,6 +2435,461 @@
       </c>
       <c r="K9" t="n">
         <v>1.65</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>50</v>
+      </c>
+      <c r="E10" t="n">
+        <v>606</v>
+      </c>
+      <c r="F10" t="n">
+        <v>462</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.3875</v>
+      </c>
+      <c r="J10" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="K10" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>8</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>36</v>
+      </c>
+      <c r="E11" t="n">
+        <v>130</v>
+      </c>
+      <c r="F11" t="n">
+        <v>97</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.4380952380952381</v>
+      </c>
+      <c r="J11" t="n">
+        <v>7.076923076923077</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2.769230769230769</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>14</v>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>70</v>
+      </c>
+      <c r="E12" t="n">
+        <v>284</v>
+      </c>
+      <c r="F12" t="n">
+        <v>219</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.1142857142857143</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.3035714285714285</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2.428571428571428</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1.928571428571429</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>14</v>
+      </c>
+      <c r="B13" t="n">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>98</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1153</v>
+      </c>
+      <c r="F13" t="n">
+        <v>885</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.06122448979591837</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.2103174603174603</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2.523809523809524</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1.619047619047619</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" t="n">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>56</v>
+      </c>
+      <c r="E14" t="n">
+        <v>355</v>
+      </c>
+      <c r="F14" t="n">
+        <v>285</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.1785714285714286</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.4047619047619048</v>
+      </c>
+      <c r="J14" t="n">
+        <v>4.857142857142857</v>
+      </c>
+      <c r="K14" t="n">
+        <v>2.095238095238095</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>8</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>126</v>
+      </c>
+      <c r="E15" t="n">
+        <v>889</v>
+      </c>
+      <c r="F15" t="n">
+        <v>660</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.04761904761904762</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.1629464285714286</v>
+      </c>
+      <c r="J15" t="n">
+        <v>2.607142857142857</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1.535714285714286</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>8</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>70</v>
+      </c>
+      <c r="E16" t="n">
+        <v>607</v>
+      </c>
+      <c r="F16" t="n">
+        <v>410</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.05714285714285714</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.3214285714285715</v>
+      </c>
+      <c r="J16" t="n">
+        <v>5.142857142857143</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1.928571428571429</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>14</v>
+      </c>
+      <c r="B17" t="n">
+        <v>8</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" t="n">
+        <v>50</v>
+      </c>
+      <c r="E17" t="n">
+        <v>667</v>
+      </c>
+      <c r="F17" t="n">
+        <v>455</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.5257731958762887</v>
+      </c>
+      <c r="J17" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K17" t="n">
+        <v>2.555555555555555</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>14</v>
+      </c>
+      <c r="B18" t="n">
+        <v>10</v>
+      </c>
+      <c r="C18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" t="n">
+        <v>48</v>
+      </c>
+      <c r="E18" t="n">
+        <v>465</v>
+      </c>
+      <c r="F18" t="n">
+        <v>299</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.04166666666666666</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.4693877551020408</v>
+      </c>
+      <c r="J18" t="n">
+        <v>9.470588235294118</v>
+      </c>
+      <c r="K18" t="n">
+        <v>2.823529411764706</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>80</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1229</v>
+      </c>
+      <c r="F19" t="n">
+        <v>821</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.296875</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2.375</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1.8125</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" t="n">
+        <v>6</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>112</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1317</v>
+      </c>
+      <c r="F20" t="n">
+        <v>968</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.01785714285714286</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.2048611111111111</v>
+      </c>
+      <c r="J20" t="n">
+        <v>2.458333333333333</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1.583333333333333</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>16</v>
+      </c>
+      <c r="B21" t="n">
+        <v>6</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" t="n">
+        <v>64</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1376</v>
+      </c>
+      <c r="F21" t="n">
+        <v>965</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.0625</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.3680555555555556</v>
+      </c>
+      <c r="J21" t="n">
+        <v>4.416666666666667</v>
+      </c>
+      <c r="K21" t="n">
+        <v>2.041666666666667</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>16</v>
+      </c>
+      <c r="B22" t="n">
+        <v>8</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>144</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1534</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1158</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.04166666666666666</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.16015625</v>
+      </c>
+      <c r="J22" t="n">
+        <v>2.5625</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>
@@ -1538,7 +2903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1874,6 +3239,500 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>10</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>90</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1184</v>
+      </c>
+      <c r="F9" t="n">
+        <v>924</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.175</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="L9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>50</v>
+      </c>
+      <c r="E10" t="n">
+        <v>940</v>
+      </c>
+      <c r="F10" t="n">
+        <v>710</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.3875</v>
+      </c>
+      <c r="J10" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="K10" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>8</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>36</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1135</v>
+      </c>
+      <c r="F11" t="n">
+        <v>721</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.2777777777777778</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.4380952380952381</v>
+      </c>
+      <c r="J11" t="n">
+        <v>7.076923076923077</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2.769230769230769</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>14</v>
+      </c>
+      <c r="B12" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>70</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1607</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1148</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.3035714285714285</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2.428571428571428</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1.928571428571429</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>14</v>
+      </c>
+      <c r="B13" t="n">
+        <v>6</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="n">
+        <v>98</v>
+      </c>
+      <c r="E13" t="n">
+        <v>52821</v>
+      </c>
+      <c r="F13" t="n">
+        <v>41031</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.2103174603174603</v>
+      </c>
+      <c r="J13" t="n">
+        <v>2.523809523809524</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1.619047619047619</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" t="n">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>56</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3186</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2087</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.4047619047619048</v>
+      </c>
+      <c r="J14" t="n">
+        <v>4.857142857142857</v>
+      </c>
+      <c r="K14" t="n">
+        <v>2.095238095238095</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>8</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
+        <v>126</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1514</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1258</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.2380952380952381</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.1629464285714286</v>
+      </c>
+      <c r="J15" t="n">
+        <v>2.607142857142857</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1.535714285714286</v>
+      </c>
+      <c r="L15" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>8</v>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="n">
+        <v>70</v>
+      </c>
+      <c r="E16" t="n">
+        <v>5687</v>
+      </c>
+      <c r="F16" t="n">
+        <v>4049</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.3214285714285715</v>
+      </c>
+      <c r="J16" t="n">
+        <v>5.142857142857143</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1.928571428571429</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>14</v>
+      </c>
+      <c r="B17" t="n">
+        <v>8</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" t="n">
+        <v>50</v>
+      </c>
+      <c r="E17" t="n">
+        <v>967</v>
+      </c>
+      <c r="F17" t="n">
+        <v>697</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.5257731958762887</v>
+      </c>
+      <c r="J17" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K17" t="n">
+        <v>2.555555555555555</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>14</v>
+      </c>
+      <c r="B18" t="n">
+        <v>10</v>
+      </c>
+      <c r="C18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" t="n">
+        <v>48</v>
+      </c>
+      <c r="E18" t="n">
+        <v>399</v>
+      </c>
+      <c r="F18" t="n">
+        <v>306</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.2916666666666667</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.4693877551020408</v>
+      </c>
+      <c r="J18" t="n">
+        <v>9.470588235294118</v>
+      </c>
+      <c r="K18" t="n">
+        <v>2.823529411764706</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>80</v>
+      </c>
+      <c r="E19" t="n">
+        <v>789</v>
+      </c>
+      <c r="F19" t="n">
+        <v>644</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.296875</v>
+      </c>
+      <c r="J19" t="n">
+        <v>2.375</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1.8125</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" t="n">
+        <v>6</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>112</v>
+      </c>
+      <c r="E20" t="n">
+        <v>51061</v>
+      </c>
+      <c r="F20" t="n">
+        <v>39769</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.2048611111111111</v>
+      </c>
+      <c r="J20" t="n">
+        <v>2.458333333333333</v>
+      </c>
+      <c r="K20" t="n">
+        <v>1.583333333333333</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>16</v>
+      </c>
+      <c r="B21" t="n">
+        <v>6</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" t="n">
+        <v>64</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1263</v>
+      </c>
+      <c r="F21" t="n">
+        <v>863</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.3680555555555556</v>
+      </c>
+      <c r="J21" t="n">
+        <v>4.416666666666667</v>
+      </c>
+      <c r="K21" t="n">
+        <v>2.041666666666667</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>